<commit_message>
Power sector calibration edits
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\elec\BPMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D687F5-129B-4F2D-84ED-A69B3782D8EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41D6A53-3CD6-41C8-8CD5-17D8956A8B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="3" r:id="rId2"/>
-    <sheet name="BPMCCS" sheetId="2" r:id="rId3"/>
+    <sheet name="Nuclear" sheetId="3" r:id="rId2"/>
+    <sheet name="Wind" sheetId="4" r:id="rId3"/>
+    <sheet name="Solar" sheetId="5" r:id="rId4"/>
+    <sheet name="BPMCCS" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Note:</t>
   </si>
@@ -176,6 +178,45 @@
   </si>
   <si>
     <t>Plans For New Reactors Worldwide</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Onshore</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Offshore</t>
+  </si>
+  <si>
+    <t>Total Onshore</t>
+  </si>
+  <si>
+    <t>Wind Europe</t>
+  </si>
+  <si>
+    <t>Wind energy in Europe</t>
+  </si>
+  <si>
+    <t>Figure A</t>
+  </si>
+  <si>
+    <t>Capacity Addition</t>
+  </si>
+  <si>
+    <t>https://proceedings.windeurope.org/biplatform/rails/active_storage/disk/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaDdDRG9JYTJWNVNTSWhNamhwZEd4ck5uTXpjMnczTW1sMmJHNWthSE0yTTNRd1ltWXpiZ1k2QmtWVU9oQmthWE53YjNOcGRHbHZia2tpQVk1cGJteHBibVU3SUdacGJHVnVZVzFsUFNKWGFXNWtSWFZ5YjNCbExWZHBibVF0Wlc1bGNtZDVMV2x1TFVWMWNtOXdaUzF6ZEdGMGFYTjBhV056TFRJd01qQXVjR1JtSWpzZ1ptbHNaVzVoYldVcVBWVlVSaTA0SnlkWGFXNWtSWFZ5YjNCbExWZHBibVF0Wlc1bGNtZDVMV2x1TFVWMWNtOXdaUzF6ZEdGMGFYTjBhV056TFRJd01qQXVjR1JtQmpzR1ZEb1JZMjl1ZEdWdWRGOTBlWEJsU1NJVVlYQndiR2xqWVhScGIyNHZjR1JtQmpzR1ZBPT0iLCJleHAiOiIyMDIxLTA5LTAxVDIyOjQ2OjAxLjcxMVoiLCJwdXIiOiJibG9iX2tleSJ9fQ==--8471a3a5562d7a916c885b3fb44c66b36966b139/WindEurope-Wind-energy-in-Europe-statistics-2020.pdf?content_type=application%2Fpdf&amp;disposition=inline%3B+filename%3D%22WindEurope-Wind-energy-in-Europe-statistics-2020.pdf%22%3B+filename%2A%3DUTF-8%27%27WindEurope-Wind-energy-in-Europe-statistics-2020.pdf</t>
+  </si>
+  <si>
+    <t>PVTech</t>
+  </si>
+  <si>
+    <t>https://www.pv-tech.org/resilient-european-solar-market-posts-double-digit-growth-in-2020/#:~:text=Despite%20the%20setbacks%20of%20COVID,in%20the%20continent%20since%202011.</t>
+  </si>
+  <si>
+    <t>Resilient' European solar market posts double-digit growth in 2020</t>
   </si>
 </sst>
 </file>
@@ -236,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,6 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -286,9 +328,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>91487</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>350520</xdr:rowOff>
+      <xdr:colOff>85137</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1270</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -313,6 +355,104 @@
         <a:xfrm>
           <a:off x="7749540" y="213361"/>
           <a:ext cx="4412027" cy="1897379"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2377</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>126395</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12504EDE-F679-4A14-B942-FF39AFBA3E51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="171450"/>
+          <a:ext cx="6380952" cy="4838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>275524</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1233D49B-878B-4080-ABE1-204ACF5BC0AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161925" y="161925"/>
+          <a:ext cx="5612699" cy="1580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -645,23 +785,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="67.1328125" customWidth="1"/>
+    <col min="2" max="2" width="67.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -669,79 +809,139 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="2"/>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -757,31 +957,31 @@
   <dimension ref="A2:AG62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.46484375" customWidth="1"/>
-    <col min="8" max="8" width="8.53125" customWidth="1"/>
-    <col min="9" max="9" width="11.86328125" customWidth="1"/>
-    <col min="10" max="10" width="32.19921875" customWidth="1"/>
-    <col min="11" max="11" width="8.46484375" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="32.1796875" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
@@ -799,9 +999,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>27</v>
@@ -821,9 +1021,9 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>27</v>
@@ -843,7 +1043,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>2023</v>
       </c>
@@ -865,9 +1065,9 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
@@ -887,9 +1087,9 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
@@ -908,9 +1108,9 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>41</v>
@@ -932,35 +1132,35 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>2018</v>
       </c>
@@ -1061,38 +1261,37 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>0</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="5">
-        <f>F5+F10</f>
-        <v>2081.4499999999998</v>
-      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="5">
-        <f>F6</f>
-        <v>447.45</v>
+        <f>E5</f>
+        <v>471</v>
       </c>
       <c r="E16" s="5">
-        <v>0</v>
+        <f>E10</f>
+        <v>1720</v>
       </c>
       <c r="F16">
-        <f>F7</f>
-        <v>1662.5</v>
+        <f>F6+F7</f>
+        <v>2109.9499999999998</v>
       </c>
       <c r="G16">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>F9</f>
-        <v>1634</v>
+        <f>E8</f>
+        <v>1720</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <f>E9</f>
+        <v>1720</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1164,322 +1363,322 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -1497,6 +1696,206 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026A5C1-A507-41BC-96F8-0D98E825E8FF}">
+  <dimension ref="A30:P35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>1493</v>
+      </c>
+      <c r="C30">
+        <v>219</v>
+      </c>
+      <c r="I30">
+        <v>706</v>
+      </c>
+      <c r="L30">
+        <v>483</v>
+      </c>
+      <c r="P30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>486</v>
+      </c>
+      <c r="C31">
+        <v>1431</v>
+      </c>
+      <c r="D31">
+        <v>1532</v>
+      </c>
+      <c r="E31">
+        <v>1400</v>
+      </c>
+      <c r="F31">
+        <v>1318</v>
+      </c>
+      <c r="G31">
+        <v>1224</v>
+      </c>
+      <c r="H31">
+        <v>1007</v>
+      </c>
+      <c r="I31">
+        <v>152</v>
+      </c>
+      <c r="J31">
+        <v>731</v>
+      </c>
+      <c r="K31">
+        <v>713</v>
+      </c>
+      <c r="L31">
+        <v>115</v>
+      </c>
+      <c r="M31">
+        <v>517</v>
+      </c>
+      <c r="N31">
+        <v>302</v>
+      </c>
+      <c r="O31">
+        <v>196</v>
+      </c>
+      <c r="P31">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <f>SUM(B30:B31)</f>
+        <v>1979</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:P32" si="0">SUM(C30:C31)</f>
+        <v>1650</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1532</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1318</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1007</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>858</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>731</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>713</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>598</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>302</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <f>SUM(B30:P30)</f>
+        <v>2918</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <f>SUM(B31:P31)</f>
+        <v>11812</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C29821-63E6-4862-9221-175C5F743F03}">
+  <dimension ref="A12:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <f>18.7*1000</f>
+        <v>18700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -1504,15 +1903,15 @@
   <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1616,7 +2015,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1720,7 +2119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1824,144 +2223,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
-        <f>Data!A16</f>
+        <f>Nuclear!A16</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>Data!B16</f>
+        <f>Nuclear!B16</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>Data!C16</f>
-        <v>2081.4499999999998</v>
+        <f>Nuclear!C16</f>
+        <v>0</v>
       </c>
       <c r="E4">
-        <f>Data!D16</f>
-        <v>447.45</v>
+        <f>Nuclear!D16</f>
+        <v>471</v>
       </c>
       <c r="F4">
-        <f>Data!E16</f>
-        <v>0</v>
+        <f>Nuclear!E16</f>
+        <v>1720</v>
       </c>
       <c r="G4">
-        <f>Data!F16</f>
-        <v>1662.5</v>
+        <f>Nuclear!F16</f>
+        <v>2109.9499999999998</v>
       </c>
       <c r="H4">
-        <f>Data!G16</f>
+        <f>Nuclear!G16</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>Data!H16</f>
+        <f>Nuclear!H16</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>Data!I16</f>
-        <v>1634</v>
+        <f>Nuclear!I16</f>
+        <v>1720</v>
       </c>
       <c r="K4">
-        <f>Data!J16</f>
-        <v>0</v>
+        <f>Nuclear!J16</f>
+        <v>1720</v>
       </c>
       <c r="L4">
-        <f>Data!K16</f>
+        <f>Nuclear!K16</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>Data!L16</f>
+        <f>Nuclear!L16</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>Data!M16</f>
+        <f>Nuclear!M16</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>Data!N16</f>
+        <f>Nuclear!N16</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>Data!O16</f>
+        <f>Nuclear!O16</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>Data!P16</f>
+        <f>Nuclear!P16</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>Data!Q16</f>
+        <f>Nuclear!Q16</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>Data!R16</f>
+        <f>Nuclear!R16</f>
         <v>0</v>
       </c>
       <c r="T4">
-        <f>Data!S16</f>
+        <f>Nuclear!S16</f>
         <v>0</v>
       </c>
       <c r="U4">
-        <f>Data!T16</f>
+        <f>Nuclear!T16</f>
         <v>0</v>
       </c>
       <c r="V4">
-        <f>Data!U16</f>
+        <f>Nuclear!U16</f>
         <v>0</v>
       </c>
       <c r="W4">
-        <f>Data!V16</f>
+        <f>Nuclear!V16</f>
         <v>0</v>
       </c>
       <c r="X4">
-        <f>Data!W16</f>
+        <f>Nuclear!W16</f>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f>Data!X16</f>
+        <f>Nuclear!X16</f>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f>Data!Y16</f>
+        <f>Nuclear!Y16</f>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f>Data!Z16</f>
+        <f>Nuclear!Z16</f>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f>Data!AA16</f>
+        <f>Nuclear!AA16</f>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f>Data!AB16</f>
+        <f>Nuclear!AB16</f>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f>Data!AC16</f>
+        <f>Nuclear!AC16</f>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>Data!AD16</f>
+        <f>Nuclear!AD16</f>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f>Data!AE16</f>
+        <f>Nuclear!AE16</f>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>Data!AF16</f>
+        <f>Nuclear!AF16</f>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f>Data!AG16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+        <f>Nuclear!AG16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2065,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2076,7 +2475,8 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f>Wind!B35</f>
+        <v>11812</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2169,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2180,7 +2580,8 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>Solar!B12</f>
+        <v>18700</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2273,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2377,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2481,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2585,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2689,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2793,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2897,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2908,7 +3309,8 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f>Wind!B34</f>
+        <v>2918</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -3001,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3105,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3209,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Data updates during calibration. 1) Updates CSC paramaters for dispatchable resources; 2) Updates BPMCCS to remove 2023 values for wind and solar, as the model is buidling sufficient resources to match historicals.
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BPMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\European Union\Models\eps-eu\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6393CE51-4E7B-431A-8EE1-3FE0470D64BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E15A3B5-27FC-4A1D-95FB-2A5C380FA813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="2280" windowWidth="22425" windowHeight="12360" firstSheet="3" activeTab="6" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -6505,26 +6505,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392E0EDE-E56C-4DF9-9C8D-7B6714D2C68A}">
   <dimension ref="B11:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="48"/>
-    <col min="3" max="3" width="46.54296875" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="48"/>
+    <col min="1" max="2" width="10.85546875" style="48"/>
+    <col min="3" max="3" width="46.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="48"/>
   </cols>
   <sheetData>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>1</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>4</v>
@@ -6544,7 +6544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
         <v>6</v>
@@ -6553,7 +6553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>8</v>
@@ -6562,7 +6562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
         <v>12</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
         <v>12</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="9" t="s">
         <v>146</v>
       </c>
@@ -6594,85 +6594,85 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="49"/>
       <c r="C22" s="50"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="132" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="50"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="132" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="50"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="132" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="50"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="132" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="50"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="132" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="50"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="132" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="50"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="132" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="50"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C30" s="50"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="132" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="132"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="132"/>
       <c r="C32" s="156" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="132"/>
       <c r="C33" s="156" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="132"/>
       <c r="C34" s="156" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
     </row>
@@ -6702,12 +6702,12 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="M1" s="57"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>27</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>28</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>9900</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>141569.94696716909</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>31</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>15844</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>33</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>63889</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>34</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>36</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>12760.4457</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>37</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>38</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>39</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>4022</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
         <v>40</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>13638</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>41</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>42</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>11612.976000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>43</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>44</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>45</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="78" t="s">
         <v>46</v>
       </c>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="M19" s="82"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>47</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>66193</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
         <v>48</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>64719.832999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
         <v>49</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>16853.470267169079</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="83" t="s">
         <v>50</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>124716.4767</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="93" t="s">
         <v>51</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>23081</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="93" t="s">
         <v>52</v>
       </c>
@@ -7671,13 +7671,13 @@
         <v>40808</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
@@ -7685,56 +7685,56 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="87" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="88" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="89" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="90" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="91" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="92" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="95" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="98" t="s">
         <v>63</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="100" t="s">
         <v>65</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>0.88562074635559918</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="100" t="s">
         <v>66</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>4.1196292554878007E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="102" t="s">
         <v>67</v>
       </c>
@@ -7766,21 +7766,21 @@
         <v>7.3182961089522852E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="97" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="96"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>70</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -7834,14 +7834,14 @@
       <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.81640625" customWidth="1"/>
-    <col min="4" max="33" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="33" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="104" t="s">
         <v>73</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
         <v>74</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>12760.4457</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="116" t="s">
         <v>75</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
         <v>49</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>16853.470267169079</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="116" t="s">
         <v>50</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>124716.4767</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">
         <v>76</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="116" t="s">
         <v>77</v>
       </c>
@@ -8524,7 +8524,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="116" t="s">
         <v>78</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>23097</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="116" t="s">
         <v>79</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>11612.976000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="116" t="s">
         <v>48</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>64719.832999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="116" t="s">
         <v>80</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>4022</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="116" t="s">
         <v>81</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>15844</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="116" t="s">
         <v>82</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>13638</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="116" t="s">
         <v>83</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>141569.94696716909</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="116" t="s">
         <v>84</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="116" t="s">
         <v>85</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>9900</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="116" t="s">
         <v>86</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>50234</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="116" t="s">
         <v>87</v>
       </c>
@@ -9599,7 +9599,7 @@
         <v>5254</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="116" t="s">
         <v>88</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>63889</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="116" t="s">
         <v>89</v>
       </c>
@@ -9801,7 +9801,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="116" t="s">
         <v>65</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="116" t="s">
         <v>66</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="125" t="s">
         <v>67</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="125" t="s">
         <v>90</v>
       </c>
@@ -10205,7 +10205,7 @@
         <v>23081</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="125" t="s">
         <v>91</v>
       </c>
@@ -10306,55 +10306,55 @@
         <v>40808</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>92</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>93</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="87" t="s">
         <v>94</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -10375,15 +10375,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" customWidth="1"/>
-    <col min="3" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="32" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="32" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>95</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>-3658.0599999999977</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -10868,7 +10868,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -10997,7 +10997,7 @@
         <v>9539.5999999999985</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>97</v>
       </c>
@@ -11126,7 +11126,7 @@
         <v>9499</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -11255,7 +11255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -11384,7 +11384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -11513,7 +11513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -11771,7 +11771,7 @@
         <v>1518.1999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -11900,7 +11900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>98</v>
       </c>
@@ -12287,7 +12287,7 @@
         <v>3338.2000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>99</v>
       </c>
@@ -12416,7 +12416,7 @@
         <v>180.20000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>100</v>
       </c>
@@ -12545,7 +12545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>101</v>
       </c>
@@ -12674,7 +12674,7 @@
         <v>2977.5999999999985</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>102</v>
       </c>
@@ -12803,17 +12803,17 @@
         <v>6521.4000000000015</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B21" s="13"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>104</v>
       </c>
@@ -12840,22 +12840,22 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.54296875" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="15.7265625" customWidth="1"/>
-    <col min="16" max="16" width="37.81640625" customWidth="1"/>
-    <col min="19" max="20" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="37.85546875" customWidth="1"/>
+    <col min="19" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>105</v>
       </c>
@@ -12873,7 +12873,7 @@
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>109</v>
       </c>
@@ -12907,7 +12907,7 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2012</v>
       </c>
@@ -12960,7 +12960,7 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -13070,7 +13070,7 @@
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -13128,7 +13128,7 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="27"/>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
@@ -13152,7 +13152,7 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K9" s="27"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -13167,7 +13167,7 @@
       <c r="X9" s="31"/>
       <c r="Y9" s="31"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -13190,7 +13190,7 @@
       <c r="X10" s="31"/>
       <c r="Y10" s="31"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="P11" s="3" t="s">
         <v>116</v>
       </c>
@@ -13201,10 +13201,10 @@
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="V12" s="31"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
@@ -13215,7 +13215,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>117</v>
       </c>
@@ -13255,7 +13255,7 @@
       <c r="W14" s="27"/>
       <c r="X14" s="27"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -13309,7 +13309,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -13361,7 +13361,7 @@
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -13413,7 +13413,7 @@
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="J18" s="36" t="s">
         <v>118</v>
       </c>
@@ -13425,13 +13425,13 @@
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="P19" s="3"/>
       <c r="X19" s="27"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>119</v>
       </c>
@@ -13443,7 +13443,7 @@
       <c r="P20" s="3"/>
       <c r="X20" s="27"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>120</v>
       </c>
@@ -13454,7 +13454,7 @@
       <c r="F21" s="26"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>121</v>
       </c>
@@ -13466,7 +13466,7 @@
       <c r="P22" s="3"/>
       <c r="S22" s="154"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
       <c r="D23" s="26"/>
@@ -13474,7 +13474,7 @@
       <c r="F23" s="26"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="26"/>
@@ -13482,19 +13482,19 @@
       <c r="F24" s="26"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
     </row>
-    <row r="27" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P27" s="40" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>123</v>
       </c>
@@ -13532,7 +13532,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>124</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>710642</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P30" s="23" t="s">
         <v>89</v>
       </c>
@@ -13611,7 +13611,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P31" s="23" t="s">
         <v>113</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>712963</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P32" s="23" t="s">
         <v>115</v>
       </c>
@@ -13695,7 +13695,7 @@
         <v>85545</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P33" s="28" t="s">
         <v>116</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>396365</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N34" s="13" t="s">
         <v>125</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>91485</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="137" t="s">
         <v>126</v>
       </c>
@@ -13822,7 +13822,7 @@
         <v>12285</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="138"/>
       <c r="B36" s="139"/>
       <c r="C36" s="138"/>
@@ -13862,7 +13862,7 @@
         <v>37320</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="140" t="s">
         <v>13</v>
       </c>
@@ -13891,7 +13891,7 @@
       <c r="AA37" s="82"/>
       <c r="AB37" s="82"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="141" t="s">
         <v>110</v>
       </c>
@@ -13934,7 +13934,7 @@
       <c r="AA38" s="82"/>
       <c r="AB38" s="82"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="145" t="s">
         <v>88</v>
       </c>
@@ -13969,7 +13969,7 @@
       <c r="AA39" s="82"/>
       <c r="AB39" s="82"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="145" t="s">
         <v>89</v>
       </c>
@@ -14004,7 +14004,7 @@
       <c r="AA40" s="82"/>
       <c r="AB40" s="82"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="145" t="s">
         <v>113</v>
       </c>
@@ -14049,7 +14049,7 @@
       <c r="AA41" s="82"/>
       <c r="AB41" s="82"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="145" t="s">
         <v>115</v>
       </c>
@@ -14094,7 +14094,7 @@
       <c r="AA42" s="82"/>
       <c r="AB42" s="82"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="147" t="s">
         <v>116</v>
       </c>
@@ -14139,7 +14139,7 @@
       <c r="AA43" s="82"/>
       <c r="AB43" s="82"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="138"/>
       <c r="B44" s="138"/>
       <c r="C44" s="138"/>
@@ -14166,7 +14166,7 @@
       <c r="AA44" s="82"/>
       <c r="AB44" s="82"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="151" t="s">
         <v>128</v>
       </c>
@@ -14193,7 +14193,7 @@
       <c r="AA45" s="82"/>
       <c r="AB45" s="82"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="141" t="s">
         <v>110</v>
       </c>
@@ -14236,7 +14236,7 @@
       <c r="AA46" s="82"/>
       <c r="AB46" s="82"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="145" t="s">
         <v>88</v>
       </c>
@@ -14269,7 +14269,7 @@
       <c r="AA47" s="82"/>
       <c r="AB47" s="82"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="145" t="s">
         <v>89</v>
       </c>
@@ -14302,7 +14302,7 @@
       <c r="AA48" s="82"/>
       <c r="AB48" s="82"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="145" t="s">
         <v>113</v>
       </c>
@@ -14345,7 +14345,7 @@
       <c r="AA49" s="82"/>
       <c r="AB49" s="82"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="145" t="s">
         <v>115</v>
       </c>
@@ -14388,7 +14388,7 @@
       <c r="AA50" s="82"/>
       <c r="AB50" s="82"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="147" t="s">
         <v>116</v>
       </c>
@@ -14431,7 +14431,7 @@
       <c r="AA51" s="82"/>
       <c r="AB51" s="82"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="O52" s="82"/>
       <c r="P52" s="136"/>
       <c r="Q52" s="136"/>
@@ -14447,7 +14447,7 @@
       <c r="AA52" s="82"/>
       <c r="AB52" s="82"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P53" s="51"/>
       <c r="Q53" s="52"/>
       <c r="R53" s="52"/>
@@ -14458,7 +14458,7 @@
       <c r="W53" s="52"/>
       <c r="X53" s="52"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P54" s="51"/>
       <c r="Q54" s="52"/>
       <c r="R54" s="52"/>
@@ -14469,7 +14469,7 @@
       <c r="W54" s="52"/>
       <c r="X54" s="52"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P55" s="51"/>
       <c r="Q55" s="52"/>
       <c r="R55" s="52"/>
@@ -14480,7 +14480,7 @@
       <c r="W55" s="52"/>
       <c r="X55" s="52"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P56" s="51"/>
       <c r="Q56" s="52"/>
       <c r="R56" s="52"/>
@@ -14491,7 +14491,7 @@
       <c r="W56" s="52"/>
       <c r="X56" s="52"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P57" s="51"/>
       <c r="Q57" s="52"/>
       <c r="R57" s="52"/>
@@ -14502,7 +14502,7 @@
       <c r="W57" s="52"/>
       <c r="X57" s="52"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P58" s="51"/>
       <c r="Q58" s="52"/>
       <c r="R58" s="52"/>
@@ -14513,7 +14513,7 @@
       <c r="W58" s="52"/>
       <c r="X58" s="52"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P59" s="51"/>
       <c r="Q59" s="52"/>
       <c r="R59" s="52"/>
@@ -14524,7 +14524,7 @@
       <c r="W59" s="52"/>
       <c r="X59" s="52"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P60" s="51"/>
       <c r="Q60" s="52"/>
       <c r="R60" s="52"/>
@@ -14555,12 +14555,12 @@
       <selection activeCell="B7" sqref="B7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -14691,7 +14691,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -14820,7 +14820,7 @@
         <v>710642</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -15054,7 +15054,7 @@
         <v>712963</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -15183,7 +15183,7 @@
         <v>85545</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>396365</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -15445,7 +15445,7 @@
         <v>291363.21999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -15578,23 +15578,23 @@
         <v>419278.77999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="97" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="96"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
@@ -15626,7 +15626,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -15661,7 +15661,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -15696,12 +15696,12 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>94</v>
       </c>
@@ -15722,16 +15722,16 @@
   </sheetPr>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -15829,7 +15829,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -15927,7 +15927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>100</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>134</v>
       </c>
@@ -16123,7 +16123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -16221,7 +16221,7 @@
         <v>3658</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -16348,7 +16348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -16364,9 +16364,8 @@
         <f>-'Retirements from BCRbQ'!D6</f>
         <v>14122</v>
       </c>
-      <c r="E7" s="7">
-        <f>'RE projections'!F8-'RE projections'!E8</f>
-        <v>7464</v>
+      <c r="E7" s="17">
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -16450,7 +16449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>101</v>
       </c>
@@ -16466,9 +16465,8 @@
         <f>-'Retirements from BCRbQ'!D19</f>
         <v>12230.48000000001</v>
       </c>
-      <c r="E8" s="7">
-        <f>'RE projections'!F9-'RE projections'!E9</f>
-        <v>10011.882499999992</v>
+      <c r="E8" s="17">
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -16552,7 +16550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -16678,7 +16676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -16776,7 +16774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -16874,7 +16872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>135</v>
       </c>
@@ -16972,7 +16970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>99</v>
       </c>
@@ -17070,7 +17068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -17168,7 +17166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -17277,7 +17275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -17375,7 +17373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>136</v>
       </c>
@@ -17473,7 +17471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -17574,7 +17572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>137</v>
       </c>
@@ -17672,7 +17670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>138</v>
       </c>
@@ -17770,7 +17768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>139</v>
       </c>
@@ -17868,7 +17866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>140</v>
       </c>
@@ -17966,7 +17964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>141</v>
       </c>
@@ -18064,7 +18062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="155" t="s">
         <v>142</v>
       </c>
@@ -18162,7 +18160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="155" t="s">
         <v>143</v>
       </c>
@@ -18260,20 +18258,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
         <v>145</v>
       </c>
@@ -18284,26 +18282,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -18526,26 +18504,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9018DBB-89A9-42C8-9D08-D8AEBFC4B055}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8E4B59-49AD-4EDF-A9EB-8EA8346AF5F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18562,4 +18541,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9018DBB-89A9-42C8-9D08-D8AEBFC4B055}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Calibrate historical solar capacity
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80099E8E-6330-4472-9FC0-D99B10708E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D846F7FA-80A0-43C9-85AA-056270405EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3710" yWindow="260" windowWidth="13490" windowHeight="11110" firstSheet="3" activeTab="6" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
+    <workbookView xWindow="44145" yWindow="3405" windowWidth="21600" windowHeight="12525" firstSheet="3" activeTab="6" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -16440,7 +16440,7 @@
         <v>15000</v>
       </c>
       <c r="E8" s="17">
-        <v>1500</v>
+        <v>12000</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -18261,6 +18261,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
@@ -18269,15 +18278,6 @@
     <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18504,20 +18504,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9018DBB-89A9-42C8-9D08-D8AEBFC4B055}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updates 2024 solar deployment to match Solar Power Europe medium scenario
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D846F7FA-80A0-43C9-85AA-056270405EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EBE8A7-D943-4D6C-BA06-B3D89B05A8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44145" yWindow="3405" windowWidth="21600" windowHeight="12525" firstSheet="3" activeTab="6" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
+    <workbookView xWindow="58800" yWindow="2070" windowWidth="21600" windowHeight="12525" firstSheet="3" activeTab="6" xr2:uid="{64B443A8-007C-42B1-80D5-84B0C57A7564}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -15726,7 +15726,7 @@
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16443,7 +16443,7 @@
         <v>12000</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>17000</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -18261,26 +18261,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -18503,10 +18483,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8E4B59-49AD-4EDF-A9EB-8EA8346AF5F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18523,20 +18534,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8E4B59-49AD-4EDF-A9EB-8EA8346AF5F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F7B5808-2083-4055-B860-939EA66F8007}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>